<commit_message>
Select grouping level and groups for time series.
</commit_message>
<xml_diff>
--- a/data/Copy of OKOKYST_Hydrografi_Stasjoner_v5.xlsx
+++ b/data/Copy of OKOKYST_Hydrografi_Stasjoner_v5.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="12" documentId="8_{7192A1F2-C0D8-4C53-B7EA-9944C0A6E4EA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{5DD803C1-C829-4807-B51E-DC1E46E31798}"/>
+  <xr:revisionPtr revIDLastSave="79" documentId="8_{7192A1F2-C0D8-4C53-B7EA-9944C0A6E4EA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{1E3AE483-321F-40E6-9C80-0B53A8D8BFA2}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="760" yWindow="760" windowWidth="14400" windowHeight="7360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CTD" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="166">
   <si>
     <t>ØKOKYST Skagerrak 2017-2020</t>
   </si>
@@ -510,6 +510,54 @@
   </si>
   <si>
     <t>Breiangen vest</t>
+  </si>
+  <si>
+    <t>VR55</t>
+  </si>
+  <si>
+    <t>Spilderbukta</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Kvænangen</t>
+  </si>
+  <si>
+    <t>VR56</t>
+  </si>
+  <si>
+    <t>VR57</t>
+  </si>
+  <si>
+    <t>Storbukta</t>
+  </si>
+  <si>
+    <t>VR58</t>
+  </si>
+  <si>
+    <t>Ullsfjorden</t>
+  </si>
+  <si>
+    <t>VR59</t>
+  </si>
+  <si>
+    <t>Reisafjorden ytre</t>
+  </si>
+  <si>
+    <t>Reisafjorden indre</t>
+  </si>
+  <si>
+    <t>Ullsfjorden/Fugløyfjorden</t>
+  </si>
+  <si>
+    <t>Sørfjorden ytre</t>
+  </si>
+  <si>
+    <t>VR4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kvænangen ytre </t>
   </si>
 </sst>
 </file>
@@ -2387,10 +2435,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{758D0152-6EA9-4C36-8FEE-81A20A52CD11}">
-  <dimension ref="A1:H39"/>
+  <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3413,6 +3461,153 @@
       </c>
       <c r="H39">
         <v>7068619</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>150</v>
+      </c>
+      <c r="B40" t="s">
+        <v>151</v>
+      </c>
+      <c r="C40" t="s">
+        <v>153</v>
+      </c>
+      <c r="D40">
+        <v>69.966399999999993</v>
+      </c>
+      <c r="E40">
+        <v>21.688700000000001</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+      <c r="G40" t="s">
+        <v>152</v>
+      </c>
+      <c r="H40" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>154</v>
+      </c>
+      <c r="B41" t="s">
+        <v>160</v>
+      </c>
+      <c r="C41" t="s">
+        <v>160</v>
+      </c>
+      <c r="D41">
+        <v>69.906800000000004</v>
+      </c>
+      <c r="E41">
+        <v>21.092700000000001</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41" t="s">
+        <v>152</v>
+      </c>
+      <c r="H41" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>155</v>
+      </c>
+      <c r="B42" t="s">
+        <v>156</v>
+      </c>
+      <c r="C42" t="s">
+        <v>161</v>
+      </c>
+      <c r="D42">
+        <v>69.851500000000001</v>
+      </c>
+      <c r="E42">
+        <v>21.1968</v>
+      </c>
+      <c r="F42">
+        <v>0</v>
+      </c>
+      <c r="G42" t="s">
+        <v>152</v>
+      </c>
+      <c r="H42" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>157</v>
+      </c>
+      <c r="B43" t="s">
+        <v>158</v>
+      </c>
+      <c r="C43" t="s">
+        <v>162</v>
+      </c>
+      <c r="D43">
+        <v>69.754400000000004</v>
+      </c>
+      <c r="E43">
+        <v>19.770099999999999</v>
+      </c>
+      <c r="F43">
+        <v>0</v>
+      </c>
+      <c r="G43" t="s">
+        <v>152</v>
+      </c>
+      <c r="H43" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>159</v>
+      </c>
+      <c r="B44" t="s">
+        <v>163</v>
+      </c>
+      <c r="C44" t="s">
+        <v>163</v>
+      </c>
+      <c r="D44">
+        <v>69.571100000000001</v>
+      </c>
+      <c r="E44">
+        <v>19.718499999999999</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
+      </c>
+      <c r="G44" t="s">
+        <v>152</v>
+      </c>
+      <c r="H44" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>164</v>
+      </c>
+      <c r="B45" t="s">
+        <v>165</v>
+      </c>
+      <c r="C45" t="s">
+        <v>153</v>
+      </c>
+      <c r="D45">
+        <v>70.116100000000003</v>
+      </c>
+      <c r="E45">
+        <v>21.072500000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>